<commit_message>
for a new file
</commit_message>
<xml_diff>
--- a/data_analyzed/Distance (miles)/Distance (miles)_games.xlsx
+++ b/data_analyzed/Distance (miles)/Distance (miles)_games.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:AF51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,114 +441,236 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Alexis Rainey</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Balduzzi</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Burns</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Curley</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Daud</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>DeLeo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Diedrichsen</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Doyle</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Espona</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Ferriolo</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Forman</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Hackman</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Hartsch</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Holzman</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Hughes</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>LaCroix</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Larripa</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>McCann</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>McFadden</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Medico</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Myers</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Pla</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Reilly</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Ricci</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Rodrigo</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Smyth</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Streib</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Tollaksen</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Wasyliw</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Yanovich</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44799</v>
       </c>
       <c r="B2" t="n">
+        <v>3.2819</v>
+      </c>
+      <c r="C2" t="n">
         <v>4.7744</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>1.8202</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>1.5278</v>
-      </c>
+      <c r="E2" t="n">
+        <v>1.8102</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="n">
+        <v>3.6881</v>
+      </c>
       <c r="J2" t="n">
+        <v>4.2564</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1.5278</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>3.6486</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="n">
+        <v>4.5392</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.8648</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>3.3876</v>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="n">
         <v>2.9987</v>
       </c>
-      <c r="K2" t="n">
+      <c r="U2" t="n">
+        <v>2.8337</v>
+      </c>
+      <c r="V2" t="n">
         <v>1.6886</v>
       </c>
-      <c r="L2" t="n">
+      <c r="W2" t="n">
+        <v>3.2401</v>
+      </c>
+      <c r="X2" t="n">
         <v>4.1089</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
+      <c r="Y2" t="n">
+        <v>2.2019</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="n">
         <v>5.0949</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="n">
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
+        <v>5.0496</v>
+      </c>
+      <c r="AE2" t="n">
         <v>3.6733</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>3.6089</v>
       </c>
     </row>
     <row r="3">
@@ -556,35 +678,75 @@
         <v>44801</v>
       </c>
       <c r="B3" t="n">
+        <v>5.2136</v>
+      </c>
+      <c r="C3" t="n">
         <v>6.2634</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>1.6608</v>
       </c>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>5.0994</v>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>5.742</v>
+      </c>
       <c r="J3" t="n">
+        <v>4.8626</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5.0994</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>4.133</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="n">
+        <v>6.1674</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.1136</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>5.8609</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="n">
         <v>3.2101</v>
       </c>
-      <c r="K3" t="n">
+      <c r="U3" t="n">
+        <v>4.6233</v>
+      </c>
+      <c r="V3" t="n">
         <v>2.0294</v>
       </c>
-      <c r="L3" t="n">
+      <c r="W3" t="n">
+        <v>3.4735</v>
+      </c>
+      <c r="X3" t="n">
         <v>5.46</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
+      <c r="Y3" t="n">
+        <v>1.6385</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="n">
         <v>5.2309</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="n">
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
+        <v>6.2604</v>
+      </c>
+      <c r="AE3" t="n">
         <v>3.0244</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>3.102</v>
       </c>
     </row>
     <row r="4">
@@ -592,35 +754,75 @@
         <v>44804</v>
       </c>
       <c r="B4" t="n">
+        <v>3.2119</v>
+      </c>
+      <c r="C4" t="n">
         <v>5.7594</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>1.7353</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>0.3875</v>
-      </c>
+      <c r="E4" t="n">
+        <v>1.8871</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>6.8435</v>
+      </c>
       <c r="J4" t="n">
-        <v>3.28</v>
+        <v>4.33</v>
       </c>
       <c r="K4" t="n">
-        <v>1.4971</v>
-      </c>
-      <c r="L4" t="n">
-        <v>5.7562</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
-        <v>5.8841</v>
-      </c>
+        <v>0.3875</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>5.391</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
+        <v>1.6023</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>6.0401</v>
+      </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="U4" t="n">
+        <v>5.048</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1.4971</v>
+      </c>
+      <c r="W4" t="n">
+        <v>4.3249</v>
+      </c>
+      <c r="X4" t="n">
+        <v>5.7562</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1.5011</v>
+      </c>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="n">
+        <v>5.8841</v>
+      </c>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
+        <v>6.4077</v>
+      </c>
+      <c r="AE4" t="n">
         <v>3.2111</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>3.3887</v>
       </c>
     </row>
     <row r="5">
@@ -628,35 +830,77 @@
         <v>44808</v>
       </c>
       <c r="B5" t="n">
+        <v>3.4935</v>
+      </c>
+      <c r="C5" t="n">
         <v>5.8592</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>1.5826</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>2.2342</v>
-      </c>
+      <c r="E5" t="n">
+        <v>2.6191</v>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>6.5772</v>
+      </c>
       <c r="J5" t="n">
+        <v>4.3885</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2.2342</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>4.8891</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
+        <v>6.1993</v>
+      </c>
+      <c r="P5" t="n">
+        <v>2.0234</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>5.5846</v>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="n">
         <v>5.5145</v>
       </c>
-      <c r="K5" t="n">
+      <c r="U5" t="n">
+        <v>4.843</v>
+      </c>
+      <c r="V5" t="n">
         <v>1.9936</v>
       </c>
-      <c r="L5" t="n">
+      <c r="W5" t="n">
+        <v>3.024</v>
+      </c>
+      <c r="X5" t="n">
         <v>5.3579</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
+      <c r="Y5" t="n">
+        <v>2.7817</v>
+      </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="n">
         <v>4.7685</v>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="n">
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="n">
+        <v>6.6192</v>
+      </c>
+      <c r="AE5" t="n">
         <v>2.4843</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>4.0818</v>
       </c>
     </row>
     <row r="6">
@@ -664,313 +908,685 @@
         <v>44813</v>
       </c>
       <c r="B6" t="n">
+        <v>1.869</v>
+      </c>
+      <c r="C6" t="n">
         <v>6.047</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>1.922</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>4.5157</v>
-      </c>
+      <c r="E6" t="n">
+        <v>2.3907</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>5.9082</v>
+      </c>
       <c r="J6" t="n">
+        <v>5.0695</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4.5157</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>5.614</v>
+      </c>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
+        <v>5.3145</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2.1095</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>6.2964</v>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="n">
         <v>4.7141</v>
       </c>
-      <c r="K6" t="n">
+      <c r="U6" t="n">
+        <v>4.8595</v>
+      </c>
+      <c r="V6" t="n">
         <v>5.7301</v>
       </c>
-      <c r="L6" t="n">
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="n">
         <v>5.8776</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="n">
+      <c r="Y6" t="n">
+        <v>1.806</v>
+      </c>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="n">
         <v>4.6898</v>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="n">
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="n">
+        <v>7.0437</v>
+      </c>
+      <c r="AE6" t="n">
         <v>3.7685</v>
       </c>
+      <c r="AF6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>44815</v>
       </c>
       <c r="B7" t="n">
+        <v>2.7805</v>
+      </c>
+      <c r="C7" t="n">
         <v>5.9936</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>1.8516</v>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>2.5483</v>
-      </c>
+      <c r="E7" t="n">
+        <v>2.2515</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>6.4686</v>
+      </c>
       <c r="J7" t="n">
+        <v>4.8816</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2.5483</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>3.803</v>
+      </c>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="n">
+        <v>6.3395</v>
+      </c>
+      <c r="P7" t="n">
+        <v>2.0668</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>5.9158</v>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="n">
         <v>6.8509</v>
       </c>
-      <c r="K7" t="n">
+      <c r="U7" t="n">
+        <v>4.0084</v>
+      </c>
+      <c r="V7" t="n">
         <v>6.7141</v>
       </c>
-      <c r="L7" t="n">
+      <c r="W7" t="n">
+        <v>4.118</v>
+      </c>
+      <c r="X7" t="n">
         <v>5.6056</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
+      <c r="Y7" t="n">
+        <v>1.9057</v>
+      </c>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="n">
         <v>3.4115</v>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="n">
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="n">
+        <v>1.2427</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>6.1982</v>
+      </c>
+      <c r="AE7" t="n">
         <v>6.0859</v>
       </c>
+      <c r="AF7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>44820</v>
       </c>
       <c r="B8" t="n">
+        <v>3.4469</v>
+      </c>
+      <c r="C8" t="n">
         <v>8.0588</v>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>2.2875</v>
-      </c>
+      <c r="E8" t="n">
+        <v>3.3085</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>8.8163</v>
+      </c>
       <c r="J8" t="n">
+        <v>4.877</v>
+      </c>
+      <c r="K8" t="n">
+        <v>2.2875</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0.2558</v>
+      </c>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="n">
+        <v>4.5221</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2.8044</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>8.4368</v>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="n">
         <v>8.309200000000001</v>
       </c>
-      <c r="K8" t="n">
+      <c r="U8" t="n">
+        <v>4.959</v>
+      </c>
+      <c r="V8" t="n">
         <v>5.7655</v>
       </c>
-      <c r="L8" t="n">
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="n">
         <v>7.3774</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="n">
+      <c r="Y8" t="n">
+        <v>2.3226</v>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="n">
         <v>8.259499999999999</v>
       </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="n">
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="n">
+        <v>1.0121</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>9.0001</v>
+      </c>
+      <c r="AE8" t="n">
         <v>5.0762</v>
       </c>
+      <c r="AF8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>44822</v>
       </c>
       <c r="B9" t="n">
+        <v>0.0503</v>
+      </c>
+      <c r="C9" t="n">
         <v>6.2813</v>
       </c>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>2.1706</v>
-      </c>
+      <c r="E9" t="n">
+        <v>2.4559</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="n">
+        <v>4.97</v>
+      </c>
       <c r="J9" t="n">
+        <v>3.4853</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.1706</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>3.6027</v>
+      </c>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="n">
+        <v>4.4728</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2.195</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>6.7495</v>
+      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="n">
         <v>6.1965</v>
       </c>
-      <c r="K9" t="n">
+      <c r="U9" t="n">
+        <v>5.401</v>
+      </c>
+      <c r="V9" t="n">
         <v>4.7072</v>
       </c>
-      <c r="L9" t="n">
+      <c r="W9" t="n">
+        <v>4.9438</v>
+      </c>
+      <c r="X9" t="n">
         <v>5.5396</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="n">
+      <c r="Y9" t="n">
+        <v>2.3094</v>
+      </c>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="n">
         <v>5.8206</v>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="n">
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="n">
+        <v>1.3759</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>6.937</v>
+      </c>
+      <c r="AE9" t="n">
         <v>4.4981</v>
       </c>
+      <c r="AF9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>44827</v>
       </c>
       <c r="B10" t="n">
+        <v>5.7147</v>
+      </c>
+      <c r="C10" t="n">
         <v>6.5291</v>
       </c>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>1.688</v>
-      </c>
+      <c r="E10" t="n">
+        <v>2.0556</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>5.6215</v>
+      </c>
       <c r="J10" t="n">
+        <v>3.6666</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1.688</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>1.1347</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="n">
+        <v>4.254</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.8384</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>5.4849</v>
+      </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="n">
         <v>6.7381</v>
       </c>
-      <c r="K10" t="n">
+      <c r="U10" t="n">
+        <v>5.3919</v>
+      </c>
+      <c r="V10" t="n">
         <v>2.6967</v>
       </c>
-      <c r="L10" t="n">
+      <c r="W10" t="n">
+        <v>3.8244</v>
+      </c>
+      <c r="X10" t="n">
         <v>5.5553</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="n">
+      <c r="Y10" t="n">
+        <v>1.6544</v>
+      </c>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="n">
         <v>5.7693</v>
       </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="n">
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="n">
+        <v>1.0419</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>5.1693</v>
+      </c>
+      <c r="AE10" t="n">
         <v>3.9047</v>
       </c>
+      <c r="AF10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>44829</v>
       </c>
       <c r="B11" t="n">
+        <v>2.9121</v>
+      </c>
+      <c r="C11" t="n">
         <v>6.8323</v>
       </c>
-      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
-        <v>2.1147</v>
-      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>5.5023</v>
+      </c>
       <c r="J11" t="n">
+        <v>4.4992</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.1147</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>2.534</v>
+      </c>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="n">
+        <v>6.8943</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2.2708</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>6.8092</v>
+      </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="n">
         <v>7.8711</v>
       </c>
-      <c r="K11" t="n">
+      <c r="U11" t="n">
+        <v>3.9061</v>
+      </c>
+      <c r="V11" t="n">
         <v>6.2192</v>
       </c>
-      <c r="L11" t="n">
+      <c r="W11" t="n">
+        <v>5.4494</v>
+      </c>
+      <c r="X11" t="n">
         <v>5.9718</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="n">
+      <c r="Y11" t="n">
+        <v>2.0836</v>
+      </c>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="n">
         <v>6.562</v>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="n">
+        <v>1.4568</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>6.7592</v>
+      </c>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>44834</v>
       </c>
       <c r="B12" t="n">
+        <v>3.9505</v>
+      </c>
+      <c r="C12" t="n">
         <v>6.8066</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>2.3877</v>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>1.9077</v>
-      </c>
+      <c r="E12" t="n">
+        <v>2.4478</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>4.1226</v>
+      </c>
       <c r="J12" t="n">
+        <v>4.1873</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.9077</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>2.6471</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="n">
+        <v>7.0022</v>
+      </c>
+      <c r="P12" t="n">
+        <v>2.1326</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>6.1221</v>
+      </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="n">
         <v>6.9744</v>
       </c>
-      <c r="K12" t="n">
+      <c r="U12" t="n">
+        <v>3.8035</v>
+      </c>
+      <c r="V12" t="n">
         <v>6.1214</v>
       </c>
-      <c r="L12" t="n">
+      <c r="W12" t="n">
+        <v>5.8701</v>
+      </c>
+      <c r="X12" t="n">
         <v>5.8941</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="n">
+      <c r="Y12" t="n">
+        <v>2.0378</v>
+      </c>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="n">
         <v>5.8446</v>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="n">
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="n">
+        <v>1.0372</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>6.5819</v>
+      </c>
+      <c r="AE12" t="n">
         <v>5.5724</v>
       </c>
+      <c r="AF12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>44836</v>
       </c>
       <c r="B13" t="n">
+        <v>7.2736</v>
+      </c>
+      <c r="C13" t="n">
         <v>6.6337</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>2.6306</v>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>2.403</v>
-      </c>
+      <c r="E13" t="n">
+        <v>2.7945</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>7.2308</v>
+      </c>
       <c r="J13" t="n">
+        <v>4.9855</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2.403</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>4.1547</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="n">
+        <v>5.2202</v>
+      </c>
+      <c r="P13" t="n">
+        <v>2.5206</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>7.1495</v>
+      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="n">
         <v>7.8587</v>
       </c>
-      <c r="K13" t="n">
+      <c r="U13" t="n">
+        <v>4.5271</v>
+      </c>
+      <c r="V13" t="n">
         <v>3.3939</v>
       </c>
-      <c r="L13" t="n">
+      <c r="W13" t="n">
+        <v>3.1399</v>
+      </c>
+      <c r="X13" t="n">
         <v>5.9926</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="n">
+      <c r="Y13" t="n">
+        <v>3.3443</v>
+      </c>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="n">
         <v>6.0299</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="n">
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="n">
+        <v>1.6801</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>7.2842</v>
+      </c>
+      <c r="AE13" t="n">
         <v>4.1483</v>
       </c>
+      <c r="AF13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>44841</v>
       </c>
       <c r="B14" t="n">
+        <v>7.566</v>
+      </c>
+      <c r="C14" t="n">
         <v>6.165</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>2.6271</v>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
-        <v>2.1956</v>
-      </c>
+      <c r="E14" t="n">
+        <v>2.0404</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>6.3024</v>
+      </c>
       <c r="J14" t="n">
+        <v>3.7054</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2.1956</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>3.0239</v>
+      </c>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="P14" t="n">
+        <v>2.1146</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>5.563</v>
+      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="n">
         <v>6.7734</v>
       </c>
-      <c r="K14" t="n">
+      <c r="U14" t="n">
+        <v>4.0029</v>
+      </c>
+      <c r="V14" t="n">
         <v>2.7607</v>
       </c>
-      <c r="L14" t="n">
+      <c r="W14" t="n">
+        <v>3.8878</v>
+      </c>
+      <c r="X14" t="n">
         <v>5.7469</v>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="n">
+      <c r="Y14" t="n">
+        <v>2.1897</v>
+      </c>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="n">
         <v>5.4776</v>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="n">
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="n">
+        <v>1.1373</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>6.6494</v>
+      </c>
+      <c r="AE14" t="n">
         <v>4.4626</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>1.999</v>
       </c>
     </row>
     <row r="15">
@@ -978,35 +1594,79 @@
         <v>44843</v>
       </c>
       <c r="B15" t="n">
+        <v>6.8022</v>
+      </c>
+      <c r="C15" t="n">
         <v>6.4613</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>2.2406</v>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>2.096</v>
-      </c>
+      <c r="E15" t="n">
+        <v>2.3787</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>4.5348</v>
+      </c>
       <c r="J15" t="n">
+        <v>3.0359</v>
+      </c>
+      <c r="K15" t="n">
+        <v>2.096</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>2.7269</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="n">
+        <v>7.34</v>
+      </c>
+      <c r="P15" t="n">
+        <v>2.2906</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>6.0233</v>
+      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="n">
         <v>7.5587</v>
       </c>
-      <c r="K15" t="n">
+      <c r="U15" t="n">
+        <v>5.6865</v>
+      </c>
+      <c r="V15" t="n">
         <v>3.1437</v>
       </c>
-      <c r="L15" t="n">
+      <c r="W15" t="n">
+        <v>5.286</v>
+      </c>
+      <c r="X15" t="n">
         <v>5.7077</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="n">
+      <c r="Y15" t="n">
+        <v>1.9984</v>
+      </c>
+      <c r="Z15" t="inlineStr"/>
+      <c r="AA15" t="n">
         <v>5.7516</v>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="n">
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="n">
+        <v>1.7343</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>6.6942</v>
+      </c>
+      <c r="AE15" t="n">
         <v>3.9155</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>2.1998</v>
       </c>
     </row>
     <row r="16">
@@ -1014,71 +1674,157 @@
         <v>44848</v>
       </c>
       <c r="B16" t="n">
+        <v>4.2939</v>
+      </c>
+      <c r="C16" t="n">
         <v>5.9456</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>2.1435</v>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>2.1952</v>
-      </c>
+      <c r="E16" t="n">
+        <v>2.2007</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>5.9394</v>
+      </c>
       <c r="J16" t="n">
+        <v>3.1502</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2.1952</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="n">
+        <v>2.8148</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="n">
+        <v>5.9458</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1.7565</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>1.0709</v>
+      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="n">
         <v>6.7051</v>
       </c>
-      <c r="K16" t="n">
+      <c r="U16" t="n">
+        <v>4.5604</v>
+      </c>
+      <c r="V16" t="n">
         <v>2.5752</v>
       </c>
-      <c r="L16" t="n">
+      <c r="W16" t="n">
+        <v>3.6666</v>
+      </c>
+      <c r="X16" t="n">
         <v>5.0721</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="n">
+      <c r="Y16" t="n">
+        <v>1.6748</v>
+      </c>
+      <c r="Z16" t="inlineStr"/>
+      <c r="AA16" t="n">
         <v>5.6105</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="n">
+      <c r="AB16" t="inlineStr"/>
+      <c r="AC16" t="n">
+        <v>1.3231</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>5.6773</v>
+      </c>
+      <c r="AE16" t="n">
         <v>3.472</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>2.2864</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>44850</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="n">
         <v>6.2533</v>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>2.3691</v>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>0.9404</v>
-      </c>
+      <c r="E17" t="n">
+        <v>2.7785</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="n">
+        <v>2.4704</v>
+      </c>
       <c r="J17" t="n">
+        <v>5.2141</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9404</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="n">
+        <v>1.5652</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="n">
+        <v>6.2654</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1.7906</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>6.2837</v>
+      </c>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="n">
         <v>7.1649</v>
       </c>
-      <c r="K17" t="n">
+      <c r="U17" t="n">
+        <v>5.0551</v>
+      </c>
+      <c r="V17" t="n">
         <v>2.8406</v>
       </c>
-      <c r="L17" t="n">
+      <c r="W17" t="n">
+        <v>6.774</v>
+      </c>
+      <c r="X17" t="n">
         <v>5.14</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="n">
+      <c r="Y17" t="n">
+        <v>1.9211</v>
+      </c>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="n">
         <v>6.1346</v>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="n">
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="n">
+        <v>1.162</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>6.7075</v>
+      </c>
+      <c r="AE17" t="n">
         <v>5.8642</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>1.674</v>
       </c>
     </row>
     <row r="18">
@@ -1086,35 +1832,79 @@
         <v>44855</v>
       </c>
       <c r="B18" t="n">
+        <v>6.5418</v>
+      </c>
+      <c r="C18" t="n">
         <v>5.9647</v>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>1.6697</v>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>1.4358</v>
-      </c>
+      <c r="E18" t="n">
+        <v>1.764</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="n">
+        <v>3.9432</v>
+      </c>
       <c r="J18" t="n">
+        <v>2.8882</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1.4358</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>1.8607</v>
+      </c>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="n">
+        <v>5.5807</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.5987</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>4.8479</v>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="n">
         <v>6.768</v>
       </c>
-      <c r="K18" t="n">
+      <c r="U18" t="n">
+        <v>3.3488</v>
+      </c>
+      <c r="V18" t="n">
         <v>1.4116</v>
       </c>
-      <c r="L18" t="n">
+      <c r="W18" t="n">
+        <v>6.6597</v>
+      </c>
+      <c r="X18" t="n">
         <v>5.3138</v>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="n">
+      <c r="Y18" t="n">
+        <v>1.5478</v>
+      </c>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="n">
         <v>5.314</v>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="n">
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="n">
+        <v>0.7531</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>6.1709</v>
+      </c>
+      <c r="AE18" t="n">
         <v>3.6279</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>2.0198</v>
       </c>
     </row>
     <row r="19">
@@ -1122,35 +1912,77 @@
         <v>44862</v>
       </c>
       <c r="B19" t="n">
+        <v>6.1462</v>
+      </c>
+      <c r="C19" t="n">
         <v>6.8101</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>2.1772</v>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>3.3896</v>
-      </c>
+      <c r="E19" t="n">
+        <v>2.8152</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="n">
+        <v>5.7589</v>
+      </c>
       <c r="J19" t="n">
+        <v>2.173</v>
+      </c>
+      <c r="K19" t="n">
+        <v>3.3896</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="n">
+        <v>0.7288</v>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="n">
+        <v>7.4024</v>
+      </c>
+      <c r="P19" t="n">
+        <v>2.0094</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>5.604</v>
+      </c>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="n">
         <v>7.514</v>
       </c>
-      <c r="K19" t="n">
+      <c r="U19" t="n">
+        <v>3.7349</v>
+      </c>
+      <c r="V19" t="n">
         <v>1.918</v>
       </c>
-      <c r="L19" t="n">
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="n">
         <v>6.1358</v>
       </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="n">
+      <c r="Y19" t="n">
+        <v>1.8517</v>
+      </c>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="n">
         <v>6.3158</v>
       </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="n">
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="n">
+        <v>1.4499</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>6.9756</v>
+      </c>
+      <c r="AE19" t="n">
         <v>4.1767</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>1.7968</v>
       </c>
     </row>
     <row r="20">
@@ -1158,1126 +1990,1906 @@
         <v>44864</v>
       </c>
       <c r="B20" t="n">
+        <v>6.9323</v>
+      </c>
+      <c r="C20" t="n">
         <v>6.8778</v>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>2.2929</v>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="n">
-        <v>1.9451</v>
-      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="n">
+        <v>4.3051</v>
+      </c>
       <c r="J20" t="n">
+        <v>2.2189</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.9451</v>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>0.4865</v>
+      </c>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="n">
+        <v>7.2457</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1.7655</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>5.2665</v>
+      </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="n">
         <v>7.0404</v>
       </c>
-      <c r="K20" t="n">
+      <c r="U20" t="n">
+        <v>4.2768</v>
+      </c>
+      <c r="V20" t="n">
         <v>2.6705</v>
       </c>
-      <c r="L20" t="n">
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="n">
         <v>6.3675</v>
       </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="n">
+      <c r="Y20" t="n">
+        <v>1.8771</v>
+      </c>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="n">
         <v>6.6561</v>
       </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="n">
+      <c r="AB20" t="inlineStr"/>
+      <c r="AC20" t="n">
+        <v>2.1679</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>6.5868</v>
+      </c>
+      <c r="AE20" t="n">
         <v>5.0594</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>1.7538</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>45010</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="n">
         <v>6.299</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>4.1799</v>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>5.5006</v>
-      </c>
+      <c r="E21" t="n">
+        <v>2.0297</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="n">
+        <v>6.5724</v>
+      </c>
       <c r="J21" t="n">
+        <v>4.754</v>
+      </c>
+      <c r="K21" t="n">
+        <v>5.5006</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="n">
+        <v>5.5823</v>
+      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="n">
         <v>5.4494</v>
       </c>
-      <c r="K21" t="n">
+      <c r="U21" t="n">
+        <v>5.4963</v>
+      </c>
+      <c r="V21" t="n">
         <v>4.6573</v>
       </c>
-      <c r="L21" t="n">
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="n">
         <v>5.5196</v>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="n">
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="n">
         <v>5.9403</v>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="n">
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="n">
+        <v>1.818</v>
+      </c>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="n">
         <v>4.5246</v>
       </c>
+      <c r="AF21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>45017</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="n">
         <v>10.4713</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>10.3099</v>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>10.0148</v>
-      </c>
+      <c r="E22" t="n">
+        <v>3.3015</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="n">
+        <v>12.5012</v>
+      </c>
       <c r="J22" t="n">
+        <v>10.6726</v>
+      </c>
+      <c r="K22" t="n">
+        <v>10.0148</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="n">
         <v>7.8893</v>
       </c>
-      <c r="K22" t="n">
+      <c r="U22" t="n">
+        <v>10.506</v>
+      </c>
+      <c r="V22" t="n">
         <v>7.8429</v>
       </c>
-      <c r="L22" t="n">
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="n">
         <v>10.1643</v>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="n">
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="n">
         <v>10.7428</v>
       </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="n">
+      <c r="AB22" t="inlineStr"/>
+      <c r="AC22" t="n">
+        <v>3.2718</v>
+      </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="n">
         <v>0</v>
       </c>
+      <c r="AF22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>45032</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="n">
         <v>9.817600000000001</v>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>7.6095</v>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>9.2621</v>
-      </c>
+      <c r="E23" t="n">
+        <v>2.3422</v>
+      </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="n">
+        <v>10.2127</v>
+      </c>
       <c r="J23" t="n">
+        <v>9.3675</v>
+      </c>
+      <c r="K23" t="n">
+        <v>9.2621</v>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="n">
+        <v>6.6352</v>
+      </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="n">
         <v>10.6696</v>
       </c>
-      <c r="K23" t="n">
+      <c r="U23" t="n">
+        <v>7.2698</v>
+      </c>
+      <c r="V23" t="n">
         <v>6.1492</v>
       </c>
-      <c r="L23" t="n">
+      <c r="W23" t="n">
+        <v>9.086499999999999</v>
+      </c>
+      <c r="X23" t="n">
         <v>9.1455</v>
       </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="n">
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="n">
         <v>8.6158</v>
       </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="n">
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="n">
+        <v>2.8322</v>
+      </c>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="n">
         <v>6.9975</v>
       </c>
+      <c r="AF23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>45035</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="n">
         <v>3.9453</v>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>5.1885</v>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="n">
-        <v>2.8403</v>
-      </c>
+      <c r="E24" t="n">
+        <v>0.5715</v>
+      </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="n">
+        <v>5.2553</v>
+      </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
+        <v>2.8403</v>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="n">
         <v>1.1038</v>
       </c>
-      <c r="L24" t="n">
+      <c r="W24" t="n">
+        <v>3.973</v>
+      </c>
+      <c r="X24" t="n">
         <v>5.0288</v>
       </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="n">
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="n">
         <v>0.773</v>
       </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="n">
+      <c r="AB24" t="inlineStr"/>
+      <c r="AC24" t="n">
+        <v>0.3393</v>
+      </c>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="n">
         <v>0.7546</v>
       </c>
+      <c r="AF24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>45039</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="n">
         <v>6.9099</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>6.276</v>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="n">
-        <v>7.7384</v>
-      </c>
+      <c r="E25" t="n">
+        <v>1.8944</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="n">
+        <v>8.186299999999999</v>
+      </c>
       <c r="J25" t="n">
+        <v>8.1714</v>
+      </c>
+      <c r="K25" t="n">
+        <v>7.7384</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="n">
         <v>8.1699</v>
       </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="n">
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="n">
+        <v>5.5042</v>
+      </c>
+      <c r="X25" t="n">
         <v>6.4925</v>
       </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="n">
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="n">
         <v>4.6115</v>
       </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="n">
+      <c r="AB25" t="inlineStr"/>
+      <c r="AC25" t="n">
+        <v>2.3098</v>
+      </c>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="n">
         <v>7.0934</v>
       </c>
+      <c r="AF25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>45156</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="n">
         <v>6.3151</v>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>3.2795</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>5.0146</v>
+      </c>
+      <c r="G26" t="n">
         <v>2.8799</v>
       </c>
-      <c r="E26" t="n">
+      <c r="H26" t="n">
         <v>3.8533</v>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
+        <v>4.3461</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1.1093</v>
+      </c>
+      <c r="K26" t="n">
         <v>3.6962</v>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="n">
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="n">
         <v>4.9534</v>
       </c>
-      <c r="I26" t="n">
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="n">
+        <v>4.1259</v>
+      </c>
+      <c r="R26" t="n">
         <v>3.587</v>
       </c>
-      <c r="J26" t="n">
+      <c r="S26" t="n">
+        <v>6.2236</v>
+      </c>
+      <c r="T26" t="n">
         <v>5.7337</v>
       </c>
-      <c r="K26" t="n">
+      <c r="U26" t="n">
+        <v>4.018</v>
+      </c>
+      <c r="V26" t="n">
         <v>3.2437</v>
       </c>
-      <c r="L26" t="n">
+      <c r="W26" t="n">
+        <v>4.7406</v>
+      </c>
+      <c r="X26" t="n">
         <v>5.2753</v>
       </c>
-      <c r="M26" t="n">
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="n">
         <v>4.2976</v>
       </c>
-      <c r="N26" t="n">
+      <c r="AA26" t="n">
         <v>3.0772</v>
       </c>
-      <c r="O26" t="n">
+      <c r="AB26" t="n">
         <v>4.7495</v>
       </c>
-      <c r="P26" t="n">
+      <c r="AC26" t="inlineStr"/>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="n">
         <v>3.4936</v>
       </c>
+      <c r="AF26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>45159</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="n">
         <v>6.3854</v>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>2.198</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>4.4273</v>
+      </c>
+      <c r="G27" t="n">
         <v>2.2975</v>
       </c>
-      <c r="E27" t="n">
+      <c r="H27" t="n">
         <v>2.4927</v>
       </c>
-      <c r="F27" t="n">
+      <c r="I27" t="n">
+        <v>4.4668</v>
+      </c>
+      <c r="J27" t="n">
+        <v>4.6197</v>
+      </c>
+      <c r="K27" t="n">
         <v>2.2787</v>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="n">
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="n">
         <v>4.969</v>
       </c>
-      <c r="I27" t="n">
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="n">
+        <v>4.7875</v>
+      </c>
+      <c r="R27" t="n">
         <v>2.414</v>
       </c>
-      <c r="J27" t="n">
+      <c r="S27" t="n">
+        <v>6.6693</v>
+      </c>
+      <c r="T27" t="n">
         <v>6.381</v>
       </c>
-      <c r="K27" t="n">
+      <c r="U27" t="n">
+        <v>2.9537</v>
+      </c>
+      <c r="V27" t="n">
         <v>3.1575</v>
       </c>
-      <c r="L27" t="n">
+      <c r="W27" t="n">
+        <v>4.8921</v>
+      </c>
+      <c r="X27" t="n">
         <v>4.7131</v>
       </c>
-      <c r="M27" t="n">
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="n">
         <v>4.3596</v>
       </c>
-      <c r="N27" t="n">
+      <c r="AA27" t="n">
         <v>4.6765</v>
       </c>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="n">
+      <c r="AB27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="n">
         <v>2.249</v>
       </c>
+      <c r="AF27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>45163</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="n">
         <v>6.4067</v>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>2.2216</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>7.0839</v>
+      </c>
+      <c r="G28" t="n">
         <v>2.2651</v>
       </c>
-      <c r="E28" t="n">
+      <c r="H28" t="n">
         <v>2.1726</v>
       </c>
-      <c r="F28" t="n">
+      <c r="I28" t="n">
+        <v>6.2683</v>
+      </c>
+      <c r="J28" t="n">
+        <v>4.2842</v>
+      </c>
+      <c r="K28" t="n">
         <v>1.9481</v>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="n">
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="n">
         <v>6.408</v>
       </c>
-      <c r="I28" t="n">
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="n">
+        <v>5.8006</v>
+      </c>
+      <c r="R28" t="n">
         <v>2.8852</v>
       </c>
-      <c r="J28" t="n">
+      <c r="S28" t="n">
+        <v>6.8971</v>
+      </c>
+      <c r="T28" t="n">
         <v>6.6763</v>
       </c>
-      <c r="K28" t="n">
+      <c r="U28" t="n">
+        <v>2.8088</v>
+      </c>
+      <c r="V28" t="n">
         <v>2.9608</v>
       </c>
-      <c r="L28" t="n">
+      <c r="W28" t="n">
+        <v>4.3549</v>
+      </c>
+      <c r="X28" t="n">
         <v>5.5827</v>
       </c>
-      <c r="M28" t="n">
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="n">
         <v>4.3821</v>
       </c>
-      <c r="N28" t="n">
+      <c r="AA28" t="n">
         <v>5.9908</v>
       </c>
-      <c r="O28" t="n">
+      <c r="AB28" t="n">
         <v>5.3136</v>
       </c>
-      <c r="P28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>45165</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="n">
         <v>6.2537</v>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="n">
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>6.8297</v>
+      </c>
+      <c r="G29" t="n">
         <v>2.5281</v>
       </c>
-      <c r="E29" t="n">
+      <c r="H29" t="n">
         <v>2.3792</v>
       </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
+        <v>2.8629</v>
+      </c>
+      <c r="J29" t="n">
+        <v>4.7517</v>
+      </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="n">
         <v>5.4501</v>
       </c>
-      <c r="I29" t="n">
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="n">
+        <v>5.4745</v>
+      </c>
+      <c r="R29" t="n">
         <v>2.4249</v>
       </c>
-      <c r="J29" t="n">
+      <c r="S29" t="n">
+        <v>7.0845</v>
+      </c>
+      <c r="T29" t="n">
         <v>6.8875</v>
       </c>
-      <c r="K29" t="n">
+      <c r="U29" t="n">
+        <v>3.7693</v>
+      </c>
+      <c r="V29" t="n">
         <v>4.7767</v>
       </c>
-      <c r="L29" t="n">
+      <c r="W29" t="n">
+        <v>4.7046</v>
+      </c>
+      <c r="X29" t="n">
         <v>6.037</v>
       </c>
-      <c r="M29" t="n">
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="n">
         <v>6.2401</v>
       </c>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="n">
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="n">
         <v>5.2273</v>
       </c>
-      <c r="P29" t="n">
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="n">
         <v>2.3359</v>
       </c>
+      <c r="AF29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>45170</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="n">
         <v>5.8722</v>
       </c>
-      <c r="C30" t="n">
+      <c r="D30" t="n">
         <v>1.9473</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>5.391</v>
+      </c>
+      <c r="G30" t="n">
         <v>1.7649</v>
       </c>
-      <c r="E30" t="n">
+      <c r="H30" t="n">
         <v>1.4988</v>
       </c>
-      <c r="F30" t="n">
+      <c r="I30" t="n">
+        <v>3.9508</v>
+      </c>
+      <c r="J30" t="n">
+        <v>4.6388</v>
+      </c>
+      <c r="K30" t="n">
         <v>1.47</v>
       </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="n">
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="n">
         <v>6.0607</v>
       </c>
-      <c r="I30" t="n">
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="n">
+        <v>5.2651</v>
+      </c>
+      <c r="R30" t="n">
         <v>1.5783</v>
       </c>
-      <c r="J30" t="n">
+      <c r="S30" t="n">
+        <v>6.9947</v>
+      </c>
+      <c r="T30" t="n">
         <v>6.1754</v>
       </c>
-      <c r="K30" t="n">
+      <c r="U30" t="n">
+        <v>2.6204</v>
+      </c>
+      <c r="V30" t="n">
         <v>2.3641</v>
       </c>
-      <c r="L30" t="n">
+      <c r="W30" t="n">
+        <v>3.5941</v>
+      </c>
+      <c r="X30" t="n">
         <v>6.1737</v>
       </c>
-      <c r="M30" t="n">
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="n">
         <v>5.22</v>
       </c>
-      <c r="N30" t="n">
+      <c r="AA30" t="n">
         <v>5.5123</v>
       </c>
-      <c r="O30" t="n">
+      <c r="AB30" t="n">
         <v>4.836</v>
       </c>
-      <c r="P30" t="n">
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="n">
         <v>1.9284</v>
       </c>
+      <c r="AF30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>45172</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="n">
         <v>5.8463</v>
       </c>
-      <c r="C31" t="n">
+      <c r="D31" t="n">
         <v>2.5193</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>4.4095</v>
+      </c>
+      <c r="G31" t="n">
         <v>2.1469</v>
       </c>
-      <c r="E31" t="n">
+      <c r="H31" t="n">
         <v>2.3706</v>
       </c>
-      <c r="F31" t="n">
+      <c r="I31" t="n">
+        <v>3.6426</v>
+      </c>
+      <c r="J31" t="n">
+        <v>4.6749</v>
+      </c>
+      <c r="K31" t="n">
         <v>0.2567</v>
       </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="n">
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="n">
         <v>5.3288</v>
       </c>
-      <c r="I31" t="n">
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="n">
+        <v>3.9472</v>
+      </c>
+      <c r="R31" t="n">
         <v>2.4146</v>
       </c>
-      <c r="J31" t="n">
+      <c r="S31" t="n">
+        <v>6.404</v>
+      </c>
+      <c r="T31" t="n">
         <v>5.2571</v>
       </c>
-      <c r="K31" t="n">
+      <c r="U31" t="n">
+        <v>2.8559</v>
+      </c>
+      <c r="V31" t="n">
         <v>2.7914</v>
       </c>
-      <c r="L31" t="n">
+      <c r="W31" t="n">
+        <v>5.0219</v>
+      </c>
+      <c r="X31" t="n">
         <v>5.6617</v>
       </c>
-      <c r="M31" t="n">
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="n">
         <v>6.1064</v>
       </c>
-      <c r="N31" t="n">
+      <c r="AA31" t="n">
         <v>5.3361</v>
       </c>
-      <c r="O31" t="n">
+      <c r="AB31" t="n">
         <v>5.2565</v>
       </c>
-      <c r="P31" t="n">
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="n">
         <v>2.4288</v>
       </c>
+      <c r="AF31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>45177</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="n">
         <v>4.8431</v>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="n">
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>6.2563</v>
+      </c>
+      <c r="G32" t="n">
         <v>1.7005</v>
       </c>
-      <c r="E32" t="n">
+      <c r="H32" t="n">
         <v>1.6278</v>
       </c>
-      <c r="F32" t="n">
+      <c r="I32" t="n">
+        <v>4.6948</v>
+      </c>
+      <c r="J32" t="n">
+        <v>4.8172</v>
+      </c>
+      <c r="K32" t="n">
         <v>1.7886</v>
       </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="n">
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="n">
         <v>5.7327</v>
       </c>
-      <c r="I32" t="n">
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="n">
+        <v>4.8716</v>
+      </c>
+      <c r="R32" t="n">
         <v>1.9919</v>
       </c>
-      <c r="J32" t="n">
+      <c r="S32" t="n">
+        <v>6.6562</v>
+      </c>
+      <c r="T32" t="n">
         <v>6.336</v>
       </c>
-      <c r="K32" t="n">
+      <c r="U32" t="n">
+        <v>1.6555</v>
+      </c>
+      <c r="V32" t="n">
         <v>2.3766</v>
       </c>
-      <c r="L32" t="n">
+      <c r="W32" t="n">
+        <v>2.9841</v>
+      </c>
+      <c r="X32" t="n">
         <v>5.0835</v>
       </c>
-      <c r="M32" t="n">
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="n">
         <v>5.9447</v>
       </c>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="n">
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="n">
         <v>5.0211</v>
       </c>
-      <c r="P32" t="n">
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="n">
         <v>2.3529</v>
       </c>
+      <c r="AF32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>45179</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="n">
         <v>7.0098</v>
       </c>
-      <c r="C33" t="n">
+      <c r="D33" t="n">
         <v>1.5938</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>6.5158</v>
+      </c>
+      <c r="G33" t="n">
         <v>1.7649</v>
       </c>
-      <c r="E33" t="n">
+      <c r="H33" t="n">
         <v>1.6004</v>
       </c>
-      <c r="F33" t="n">
+      <c r="I33" t="n">
+        <v>3.8618</v>
+      </c>
+      <c r="J33" t="n">
+        <v>6.1956</v>
+      </c>
+      <c r="K33" t="n">
         <v>1.6445</v>
       </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="n">
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="n">
         <v>5.8982</v>
       </c>
-      <c r="I33" t="n">
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="n">
         <v>1.8315</v>
       </c>
-      <c r="J33" t="n">
+      <c r="S33" t="n">
+        <v>6.941</v>
+      </c>
+      <c r="T33" t="n">
         <v>7.3028</v>
       </c>
-      <c r="K33" t="n">
+      <c r="U33" t="n">
+        <v>1.9222</v>
+      </c>
+      <c r="V33" t="n">
         <v>1.7337</v>
       </c>
-      <c r="L33" t="n">
+      <c r="W33" t="n">
+        <v>4.4413</v>
+      </c>
+      <c r="X33" t="n">
         <v>6.2742</v>
       </c>
-      <c r="M33" t="n">
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="n">
         <v>5.542</v>
       </c>
-      <c r="N33" t="n">
+      <c r="AA33" t="n">
         <v>5.8856</v>
       </c>
-      <c r="O33" t="n">
+      <c r="AB33" t="n">
         <v>5.4806</v>
       </c>
-      <c r="P33" t="n">
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="n">
         <v>1.9109</v>
       </c>
+      <c r="AF33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>45184</v>
       </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="n">
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="n">
         <v>0.6489</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>6.0224</v>
+      </c>
+      <c r="G34" t="n">
         <v>1.857</v>
       </c>
-      <c r="E34" t="n">
+      <c r="H34" t="n">
         <v>1.9362</v>
       </c>
-      <c r="F34" t="n">
+      <c r="I34" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="J34" t="n">
+        <v>4.9513</v>
+      </c>
+      <c r="K34" t="n">
         <v>1.8053</v>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="n">
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="n">
         <v>6.124</v>
       </c>
-      <c r="I34" t="n">
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="n">
         <v>2.1778</v>
       </c>
-      <c r="J34" t="n">
+      <c r="S34" t="n">
+        <v>5.869</v>
+      </c>
+      <c r="T34" t="n">
         <v>6.5963</v>
       </c>
-      <c r="K34" t="n">
+      <c r="U34" t="n">
+        <v>2.7746</v>
+      </c>
+      <c r="V34" t="n">
         <v>2.6118</v>
       </c>
-      <c r="L34" t="n">
+      <c r="W34" t="n">
+        <v>4.1815</v>
+      </c>
+      <c r="X34" t="n">
         <v>6.1589</v>
       </c>
-      <c r="M34" t="n">
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="n">
         <v>5.1456</v>
       </c>
-      <c r="N34" t="n">
+      <c r="AA34" t="n">
         <v>4.1411</v>
       </c>
-      <c r="O34" t="n">
+      <c r="AB34" t="n">
         <v>4.3767</v>
       </c>
-      <c r="P34" t="n">
+      <c r="AC34" t="inlineStr"/>
+      <c r="AD34" t="inlineStr"/>
+      <c r="AE34" t="n">
         <v>3.1691</v>
       </c>
+      <c r="AF34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>45186</v>
       </c>
       <c r="B35" t="inlineStr"/>
-      <c r="C35" t="n">
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="n">
         <v>1.5898</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>5.8299</v>
+      </c>
+      <c r="G35" t="n">
         <v>1.5375</v>
       </c>
-      <c r="E35" t="n">
+      <c r="H35" t="n">
         <v>1.6723</v>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
+        <v>3.1881</v>
+      </c>
+      <c r="J35" t="n">
+        <v>4.0934</v>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="n">
         <v>5.6199</v>
       </c>
-      <c r="I35" t="n">
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="n">
         <v>1.9776</v>
       </c>
-      <c r="J35" t="n">
+      <c r="S35" t="n">
+        <v>6.9232</v>
+      </c>
+      <c r="T35" t="n">
         <v>6.5452</v>
       </c>
-      <c r="K35" t="n">
+      <c r="U35" t="n">
+        <v>2.9011</v>
+      </c>
+      <c r="V35" t="n">
         <v>2.8373</v>
       </c>
-      <c r="L35" t="n">
+      <c r="W35" t="n">
+        <v>3.7303</v>
+      </c>
+      <c r="X35" t="n">
         <v>5.5766</v>
       </c>
-      <c r="M35" t="n">
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="n">
         <v>2.6244</v>
       </c>
-      <c r="N35" t="n">
+      <c r="AA35" t="n">
         <v>6.0685</v>
       </c>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="n">
+      <c r="AB35" t="inlineStr"/>
+      <c r="AC35" t="inlineStr"/>
+      <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="n">
         <v>3.3621</v>
       </c>
+      <c r="AF35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>45191</v>
       </c>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="n">
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
         <v>2.5121</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>6.3964</v>
+      </c>
+      <c r="G36" t="n">
         <v>1.5555</v>
       </c>
-      <c r="E36" t="n">
+      <c r="H36" t="n">
         <v>1.7095</v>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
+        <v>3.2575</v>
+      </c>
+      <c r="J36" t="n">
+        <v>5.2967</v>
+      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="n">
         <v>5.9071</v>
       </c>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="n">
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="n">
+        <v>5.6643</v>
+      </c>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="n">
+        <v>7.216</v>
+      </c>
+      <c r="T36" t="n">
         <v>6.6449</v>
       </c>
-      <c r="K36" t="n">
+      <c r="U36" t="n">
+        <v>3.0375</v>
+      </c>
+      <c r="V36" t="n">
         <v>3.2544</v>
       </c>
-      <c r="L36" t="n">
+      <c r="W36" t="n">
+        <v>4.5484</v>
+      </c>
+      <c r="X36" t="n">
         <v>5.3834</v>
       </c>
-      <c r="M36" t="n">
+      <c r="Y36" t="inlineStr"/>
+      <c r="Z36" t="n">
         <v>1.4113</v>
       </c>
-      <c r="N36" t="n">
+      <c r="AA36" t="n">
         <v>4.9394</v>
       </c>
-      <c r="O36" t="n">
+      <c r="AB36" t="n">
         <v>4.8335</v>
       </c>
-      <c r="P36" t="n">
+      <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="n">
         <v>2.6337</v>
       </c>
+      <c r="AF36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>45198</v>
       </c>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="n">
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="n">
         <v>2.5127</v>
       </c>
-      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>6.1779</v>
+      </c>
       <c r="G37" t="inlineStr"/>
-      <c r="H37" t="n">
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
+        <v>4.6737</v>
+      </c>
+      <c r="J37" t="n">
+        <v>5.5359</v>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="n">
         <v>6.3291</v>
       </c>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="n">
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="n">
+        <v>6.3676</v>
+      </c>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="n">
+        <v>7.1955</v>
+      </c>
+      <c r="T37" t="n">
         <v>5.6466</v>
       </c>
-      <c r="K37" t="n">
+      <c r="U37" t="n">
+        <v>2.796</v>
+      </c>
+      <c r="V37" t="n">
         <v>3.1327</v>
       </c>
-      <c r="L37" t="n">
+      <c r="W37" t="n">
+        <v>4.0612</v>
+      </c>
+      <c r="X37" t="n">
         <v>6.1591</v>
       </c>
-      <c r="M37" t="n">
+      <c r="Y37" t="inlineStr"/>
+      <c r="Z37" t="n">
         <v>7.1289</v>
       </c>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="n">
+      <c r="AA37" t="inlineStr"/>
+      <c r="AB37" t="n">
         <v>5.9526</v>
       </c>
-      <c r="P37" t="n">
+      <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="inlineStr"/>
+      <c r="AE37" t="n">
         <v>2.8751</v>
       </c>
+      <c r="AF37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>45200</v>
       </c>
       <c r="B38" t="inlineStr"/>
-      <c r="C38" t="n">
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="n">
         <v>3.956</v>
       </c>
-      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>5.5526</v>
+      </c>
       <c r="G38" t="inlineStr"/>
-      <c r="H38" t="n">
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>4.0781</v>
+      </c>
+      <c r="J38" t="n">
+        <v>2.8644</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="n">
         <v>5.9026</v>
       </c>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="n">
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="n">
+        <v>3.7166</v>
+      </c>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="n">
+        <v>6.3371</v>
+      </c>
+      <c r="T38" t="n">
         <v>5.665</v>
       </c>
-      <c r="K38" t="n">
+      <c r="U38" t="n">
+        <v>4.3847</v>
+      </c>
+      <c r="V38" t="n">
         <v>4.1854</v>
       </c>
-      <c r="L38" t="n">
+      <c r="W38" t="n">
+        <v>4.4762</v>
+      </c>
+      <c r="X38" t="n">
         <v>5.3518</v>
       </c>
-      <c r="M38" t="n">
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="n">
         <v>5.5954</v>
       </c>
-      <c r="N38" t="n">
+      <c r="AA38" t="n">
         <v>5.556</v>
       </c>
-      <c r="O38" t="n">
+      <c r="AB38" t="n">
         <v>4.3128</v>
       </c>
-      <c r="P38" t="n">
+      <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="n">
         <v>4.6146</v>
       </c>
+      <c r="AF38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>45205</v>
       </c>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="n">
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="n">
         <v>2.5549</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>6.9423</v>
+      </c>
+      <c r="G39" t="n">
         <v>2.6765</v>
       </c>
-      <c r="E39" t="n">
+      <c r="H39" t="n">
         <v>2.2039</v>
       </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
+        <v>4.1551</v>
+      </c>
+      <c r="J39" t="n">
+        <v>5.3735</v>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="n">
         <v>6.5562</v>
       </c>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="n">
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="n">
+        <v>7.0091</v>
+      </c>
+      <c r="T39" t="n">
         <v>7.2072</v>
       </c>
-      <c r="K39" t="n">
+      <c r="U39" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="V39" t="n">
         <v>2.4656</v>
       </c>
-      <c r="L39" t="n">
+      <c r="W39" t="n">
+        <v>3.4654</v>
+      </c>
+      <c r="X39" t="n">
         <v>6.0786</v>
       </c>
-      <c r="M39" t="n">
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="n">
         <v>7.3297</v>
       </c>
-      <c r="N39" t="n">
+      <c r="AA39" t="n">
         <v>6.6156</v>
       </c>
-      <c r="O39" t="n">
+      <c r="AB39" t="n">
         <v>5.9642</v>
       </c>
-      <c r="P39" t="n">
+      <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="inlineStr"/>
+      <c r="AE39" t="n">
         <v>3.3138</v>
       </c>
+      <c r="AF39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>45207</v>
       </c>
       <c r="B40" t="inlineStr"/>
-      <c r="C40" t="n">
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="n">
         <v>2.3945</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>6.3815</v>
+      </c>
+      <c r="G40" t="n">
         <v>2.0451</v>
       </c>
-      <c r="E40" t="n">
+      <c r="H40" t="n">
         <v>2.0164</v>
       </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
+        <v>2.4674</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3.6738</v>
+      </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="n">
         <v>6.0548</v>
       </c>
-      <c r="I40" t="n">
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="n">
         <v>1.8911</v>
       </c>
-      <c r="J40" t="n">
+      <c r="S40" t="n">
+        <v>7.1982</v>
+      </c>
+      <c r="T40" t="n">
         <v>6.6784</v>
       </c>
-      <c r="K40" t="n">
+      <c r="U40" t="n">
+        <v>3.0199</v>
+      </c>
+      <c r="V40" t="n">
         <v>3.5418</v>
       </c>
-      <c r="L40" t="n">
+      <c r="W40" t="n">
+        <v>4.1582</v>
+      </c>
+      <c r="X40" t="n">
         <v>6.0064</v>
       </c>
-      <c r="M40" t="n">
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="n">
         <v>7.0846</v>
       </c>
-      <c r="N40" t="n">
+      <c r="AA40" t="n">
         <v>5.9998</v>
       </c>
-      <c r="O40" t="n">
+      <c r="AB40" t="n">
         <v>5.2635</v>
       </c>
-      <c r="P40" t="n">
+      <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="n">
         <v>2.7444</v>
       </c>
+      <c r="AF40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>45212</v>
       </c>
       <c r="B41" t="inlineStr"/>
-      <c r="C41" t="n">
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="n">
         <v>2.4566</v>
       </c>
-      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>5.9427</v>
+      </c>
       <c r="G41" t="inlineStr"/>
-      <c r="H41" t="n">
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
+        <v>4.8182</v>
+      </c>
+      <c r="J41" t="n">
+        <v>4.8964</v>
+      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
         <v>5.5022</v>
       </c>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="n">
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="n">
+        <v>6.551</v>
+      </c>
+      <c r="T41" t="n">
         <v>5.6404</v>
       </c>
-      <c r="K41" t="n">
+      <c r="U41" t="n">
+        <v>3.2237</v>
+      </c>
+      <c r="V41" t="n">
         <v>3.3371</v>
       </c>
-      <c r="L41" t="n">
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="n">
         <v>6.1122</v>
       </c>
-      <c r="M41" t="n">
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="n">
         <v>6.1557</v>
       </c>
-      <c r="N41" t="n">
+      <c r="AA41" t="n">
         <v>4.8587</v>
       </c>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="n">
+      <c r="AB41" t="inlineStr"/>
+      <c r="AC41" t="inlineStr"/>
+      <c r="AD41" t="inlineStr"/>
+      <c r="AE41" t="n">
         <v>3.2979</v>
       </c>
+      <c r="AF41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>45219</v>
       </c>
       <c r="B42" t="inlineStr"/>
-      <c r="C42" t="n">
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="n">
         <v>0.2389</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>4.0689</v>
+      </c>
+      <c r="G42" t="n">
         <v>1.7261</v>
       </c>
-      <c r="E42" t="n">
+      <c r="H42" t="n">
         <v>1.9096</v>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
+        <v>2.6492</v>
+      </c>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="n">
         <v>3.8625</v>
       </c>
-      <c r="I42" t="n">
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="n">
         <v>1.7435</v>
       </c>
-      <c r="J42" t="n">
+      <c r="S42" t="n">
+        <v>4.3489</v>
+      </c>
+      <c r="T42" t="n">
         <v>4.0214</v>
       </c>
-      <c r="K42" t="n">
+      <c r="U42" t="n">
+        <v>1.7128</v>
+      </c>
+      <c r="V42" t="n">
         <v>1.5429</v>
       </c>
-      <c r="L42" t="n">
+      <c r="W42" t="n">
+        <v>2.3273</v>
+      </c>
+      <c r="X42" t="n">
         <v>3.7017</v>
       </c>
-      <c r="M42" t="n">
+      <c r="Y42" t="inlineStr"/>
+      <c r="Z42" t="n">
         <v>4.0127</v>
       </c>
-      <c r="N42" t="n">
+      <c r="AA42" t="n">
         <v>3.8832</v>
       </c>
-      <c r="O42" t="n">
+      <c r="AB42" t="n">
         <v>3.4237</v>
       </c>
-      <c r="P42" t="n">
+      <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="inlineStr"/>
+      <c r="AE42" t="n">
         <v>3.47</v>
       </c>
+      <c r="AF42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>45221</v>
       </c>
       <c r="B43" t="inlineStr"/>
-      <c r="C43" t="n">
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="n">
         <v>0.3985</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
+        <v>7.3024</v>
+      </c>
+      <c r="G43" t="n">
         <v>1.6144</v>
       </c>
-      <c r="E43" t="n">
+      <c r="H43" t="n">
         <v>1.6377</v>
       </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
+        <v>2.9476</v>
+      </c>
+      <c r="J43" t="n">
+        <v>4.925</v>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="n">
         <v>5.9346</v>
       </c>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="n">
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="n">
+        <v>6.0508</v>
+      </c>
+      <c r="T43" t="n">
         <v>6.2741</v>
       </c>
-      <c r="K43" t="n">
+      <c r="U43" t="n">
+        <v>1.9168</v>
+      </c>
+      <c r="V43" t="n">
         <v>2.4314</v>
       </c>
-      <c r="L43" t="n">
+      <c r="W43" t="n">
+        <v>1.4493</v>
+      </c>
+      <c r="X43" t="n">
         <v>5.8336</v>
       </c>
-      <c r="M43" t="n">
+      <c r="Y43" t="inlineStr"/>
+      <c r="Z43" t="n">
         <v>6.57</v>
       </c>
-      <c r="N43" t="n">
+      <c r="AA43" t="n">
         <v>6.0408</v>
       </c>
-      <c r="O43" t="n">
+      <c r="AB43" t="n">
         <v>4.8787</v>
       </c>
-      <c r="P43" t="n">
+      <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="inlineStr"/>
+      <c r="AE43" t="n">
         <v>3.1197</v>
       </c>
+      <c r="AF43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>45226</v>
       </c>
       <c r="B44" t="inlineStr"/>
-      <c r="C44" t="n">
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="n">
         <v>1.6548</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>7.5412</v>
+      </c>
+      <c r="G44" t="n">
         <v>1.6716</v>
       </c>
-      <c r="E44" t="n">
+      <c r="H44" t="n">
         <v>1.4267</v>
       </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
+        <v>2.2441</v>
+      </c>
+      <c r="J44" t="n">
+        <v>5.7927</v>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="n">
         <v>6.0918</v>
       </c>
-      <c r="I44" t="n">
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="n">
         <v>0.2233</v>
       </c>
-      <c r="J44" t="n">
+      <c r="S44" t="n">
+        <v>7.4432</v>
+      </c>
+      <c r="T44" t="n">
         <v>7.0934</v>
       </c>
-      <c r="K44" t="n">
+      <c r="U44" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="V44" t="n">
         <v>4.0715</v>
       </c>
-      <c r="L44" t="n">
+      <c r="W44" t="n">
+        <v>1.8069</v>
+      </c>
+      <c r="X44" t="n">
         <v>6.1714</v>
       </c>
-      <c r="M44" t="n">
+      <c r="Y44" t="inlineStr"/>
+      <c r="Z44" t="n">
         <v>6.9628</v>
       </c>
-      <c r="N44" t="n">
+      <c r="AA44" t="n">
         <v>6.0446</v>
       </c>
-      <c r="O44" t="n">
+      <c r="AB44" t="n">
         <v>5.8071</v>
       </c>
-      <c r="P44" t="n">
+      <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr"/>
+      <c r="AE44" t="n">
         <v>3.2048</v>
       </c>
+      <c r="AF44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>45228</v>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="n">
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="n">
         <v>1.9271</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="n">
+        <v>7.5984</v>
+      </c>
+      <c r="G45" t="n">
         <v>1.763</v>
       </c>
-      <c r="E45" t="n">
+      <c r="H45" t="n">
         <v>0.6748</v>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
+        <v>5.6895</v>
+      </c>
+      <c r="J45" t="n">
+        <v>5.6757</v>
+      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="n">
         <v>7.3396</v>
       </c>
-      <c r="I45" t="n">
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="n">
         <v>2.3511</v>
       </c>
-      <c r="J45" t="n">
+      <c r="S45" t="n">
+        <v>8.901</v>
+      </c>
+      <c r="T45" t="n">
         <v>6.0801</v>
       </c>
-      <c r="K45" t="n">
+      <c r="U45" t="n">
+        <v>2.7872</v>
+      </c>
+      <c r="V45" t="n">
         <v>4.5677</v>
       </c>
-      <c r="L45" t="n">
+      <c r="W45" t="n">
+        <v>4.3384</v>
+      </c>
+      <c r="X45" t="n">
         <v>7.4441</v>
       </c>
-      <c r="M45" t="n">
+      <c r="Y45" t="inlineStr"/>
+      <c r="Z45" t="n">
         <v>7.2367</v>
       </c>
-      <c r="N45" t="n">
+      <c r="AA45" t="n">
         <v>6.2306</v>
       </c>
-      <c r="O45" t="n">
+      <c r="AB45" t="n">
         <v>7.245</v>
       </c>
-      <c r="P45" t="n">
+      <c r="AC45" t="inlineStr"/>
+      <c r="AD45" t="inlineStr"/>
+      <c r="AE45" t="n">
         <v>4.2975</v>
       </c>
+      <c r="AF45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>45232</v>
       </c>
       <c r="B46" t="inlineStr"/>
-      <c r="C46" t="n">
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="n">
         <v>1.6798</v>
       </c>
-      <c r="D46" t="n">
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="n">
+        <v>6.309</v>
+      </c>
+      <c r="G46" t="n">
         <v>1.4011</v>
       </c>
-      <c r="E46" t="n">
+      <c r="H46" t="n">
         <v>1.6174</v>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
+        <v>4.9911</v>
+      </c>
+      <c r="J46" t="n">
+        <v>5.2091</v>
+      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="n">
         <v>5.3701</v>
       </c>
-      <c r="I46" t="n">
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="n">
         <v>1.7276</v>
       </c>
-      <c r="J46" t="n">
+      <c r="S46" t="n">
+        <v>6.5551</v>
+      </c>
+      <c r="T46" t="n">
         <v>6.472</v>
       </c>
-      <c r="K46" t="n">
+      <c r="U46" t="n">
+        <v>1.7805</v>
+      </c>
+      <c r="V46" t="n">
         <v>4.0341</v>
       </c>
-      <c r="L46" t="n">
+      <c r="W46" t="n">
+        <v>2.298</v>
+      </c>
+      <c r="X46" t="n">
         <v>5.8374</v>
       </c>
-      <c r="M46" t="n">
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="n">
         <v>4.835</v>
       </c>
-      <c r="N46" t="n">
+      <c r="AA46" t="n">
         <v>5.6589</v>
       </c>
-      <c r="O46" t="n">
+      <c r="AB46" t="n">
         <v>5.7444</v>
       </c>
-      <c r="P46" t="n">
+      <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr"/>
+      <c r="AE46" t="n">
         <v>3.0505</v>
       </c>
+      <c r="AF46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2285,87 +3897,119 @@
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
-      <c r="D47" t="n">
-        <v>5.4596</v>
-      </c>
-      <c r="E47" t="n">
-        <v>10.0664</v>
-      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
+        <v>5.4596</v>
+      </c>
+      <c r="H47" t="n">
+        <v>10.0664</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="n">
         <v>5.7861</v>
       </c>
-      <c r="H47" t="n">
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="n">
         <v>3.0498</v>
       </c>
-      <c r="I47" t="n">
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="n">
         <v>2.9315</v>
       </c>
-      <c r="J47" t="n">
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="n">
         <v>10.3599</v>
       </c>
-      <c r="K47" t="n">
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="n">
         <v>4.979</v>
       </c>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="n">
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr"/>
+      <c r="Z47" t="n">
         <v>9.925700000000001</v>
       </c>
-      <c r="N47" t="n">
+      <c r="AA47" t="n">
         <v>9.6678</v>
       </c>
-      <c r="O47" t="n">
+      <c r="AB47" t="n">
         <v>9.4741</v>
       </c>
-      <c r="P47" t="n">
+      <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="inlineStr"/>
+      <c r="AE47" t="n">
         <v>4.9569</v>
       </c>
+      <c r="AF47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>45396</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="n">
         <v>5.349</v>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
         <v>4.0114</v>
       </c>
-      <c r="E48" t="n">
+      <c r="H48" t="n">
         <v>5.4451</v>
       </c>
-      <c r="F48" t="n">
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="n">
         <v>5.019</v>
       </c>
-      <c r="G48" t="n">
+      <c r="L48" t="n">
         <v>4.7279</v>
       </c>
-      <c r="H48" t="n">
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="n">
         <v>5.3135</v>
       </c>
-      <c r="I48" t="n">
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="n">
         <v>4.31</v>
       </c>
-      <c r="J48" t="n">
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="n">
         <v>6.5401</v>
       </c>
-      <c r="K48" t="n">
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="n">
         <v>5.2735</v>
       </c>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="n">
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="n">
         <v>5.7914</v>
       </c>
-      <c r="N48" t="n">
+      <c r="AA48" t="n">
         <v>5.1631</v>
       </c>
-      <c r="O48" t="n">
+      <c r="AB48" t="n">
         <v>4.1288</v>
       </c>
-      <c r="P48" t="n">
+      <c r="AC48" t="inlineStr"/>
+      <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="n">
         <v>5.3742</v>
       </c>
+      <c r="AF48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2374,78 +4018,110 @@
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="n">
-        <v>6.9332</v>
-      </c>
-      <c r="F49" t="n">
-        <v>6.9478</v>
-      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
+        <v>6.9332</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="n">
+        <v>6.9478</v>
+      </c>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="n">
         <v>5.8607</v>
       </c>
-      <c r="I49" t="n">
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="n">
         <v>5.7628</v>
       </c>
-      <c r="J49" t="n">
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="n">
         <v>6.9594</v>
       </c>
-      <c r="K49" t="n">
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="n">
         <v>3.2225</v>
       </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="n">
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
+      <c r="Z49" t="n">
         <v>7.5683</v>
       </c>
-      <c r="N49" t="n">
+      <c r="AA49" t="n">
         <v>6.6718</v>
       </c>
-      <c r="O49" t="n">
+      <c r="AB49" t="n">
         <v>7.3675</v>
       </c>
-      <c r="P49" t="n">
+      <c r="AC49" t="inlineStr"/>
+      <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="n">
         <v>6.4692</v>
       </c>
+      <c r="AF49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>45403</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="n">
         <v>8.0427</v>
       </c>
-      <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" t="n">
-        <v>5.9788</v>
-      </c>
-      <c r="F50" t="n">
-        <v>8.370699999999999</v>
-      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
-        <v>4.6756</v>
-      </c>
-      <c r="I50" t="n">
-        <v>4.4451</v>
-      </c>
-      <c r="J50" t="n">
-        <v>6.1292</v>
-      </c>
+        <v>5.9788</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
       <c r="K50" t="n">
-        <v>4.9293</v>
+        <v>8.370699999999999</v>
       </c>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="n">
+        <v>4.6756</v>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="n">
+        <v>4.4451</v>
+      </c>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="n">
+        <v>6.1292</v>
+      </c>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="n">
+        <v>4.9293</v>
+      </c>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" t="inlineStr"/>
+      <c r="AA50" t="n">
         <v>5.3345</v>
       </c>
-      <c r="O50" t="n">
+      <c r="AB50" t="n">
         <v>8.1021</v>
       </c>
-      <c r="P50" t="n">
+      <c r="AC50" t="inlineStr"/>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="n">
         <v>4.6456</v>
       </c>
+      <c r="AF50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2454,38 +4130,54 @@
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
-      <c r="E51" t="n">
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="n">
         <v>6.9155</v>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="n">
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="n">
         <v>3.7142</v>
       </c>
-      <c r="H51" t="n">
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="n">
         <v>4.6951</v>
       </c>
-      <c r="I51" t="n">
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="n">
         <v>4.2571</v>
       </c>
-      <c r="J51" t="n">
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="n">
         <v>6.5383</v>
       </c>
-      <c r="K51" t="n">
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="n">
         <v>5.6942</v>
       </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="n">
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="n">
         <v>6.4481</v>
       </c>
-      <c r="N51" t="n">
+      <c r="AA51" t="n">
         <v>5.5971</v>
       </c>
-      <c r="O51" t="n">
+      <c r="AB51" t="n">
         <v>6.6856</v>
       </c>
-      <c r="P51" t="n">
+      <c r="AC51" t="inlineStr"/>
+      <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="n">
         <v>5.91</v>
       </c>
+      <c r="AF51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>